<commit_message>
last set of modifications
</commit_message>
<xml_diff>
--- a/bacs_site_occ.xlsx
+++ b/bacs_site_occ.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="450" windowWidth="19875" windowHeight="9120" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="510" windowWidth="19875" windowHeight="9060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="bacs_site_occ" sheetId="1" r:id="rId1"/>
     <sheet name="bacs_habi_date_time" sheetId="2" r:id="rId2"/>
     <sheet name="bacs_hab_date_time" sheetId="4" r:id="rId3"/>
     <sheet name="combinations" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">combinations!$A$4:$J$85</definedName>
@@ -1035,7 +1036,7 @@
   <dimension ref="A3:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,7 +1408,7 @@
   <dimension ref="A3:R47"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C21:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7934,4 +7935,16 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>